<commit_message>
Adicionando envio de resultado de busca de carros no ds
</commit_message>
<xml_diff>
--- a/dadosCarros.xlsx
+++ b/dadosCarros.xlsx
@@ -7,6 +7,7 @@
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Planilha1" sheetId="2" r:id="rId2"/>
+    <x:sheet name="Carros" sheetId="5" r:id="rId5"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
@@ -557,6 +558,24 @@
   </x:si>
   <x:si>
     <x:t>https://www.webmotors.com.br/comprar/ford/ka/10-ti-vct-flex-freestyle-manual/4-portas/2020-2021/59209412</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Nome</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ano</x:t>
+  </x:si>
+  <x:si>
+    <x:t>km</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Local</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Preco</x:t>
+  </x:si>
+  <x:si>
+    <x:t>URL</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -1860,4 +1879,44 @@
   <x:headerFooter/>
   <x:tableParts count="0"/>
 </x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:F1"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:6">
+      <x:c r="A1" s="0" t="s">
+        <x:v>181</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>182</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>183</x:v>
+      </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>184</x:v>
+      </x:c>
+      <x:c r="E1" s="0" t="s">
+        <x:v>185</x:v>
+      </x:c>
+      <x:c r="F1" s="0" t="s">
+        <x:v>186</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>